<commit_message>
Ajustando o tamanho de uma das colunas
</commit_message>
<xml_diff>
--- a/df_tabela.xlsx
+++ b/df_tabela.xlsx
@@ -1,105 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Furio\Desktop\Intensivao\python-basico\Etl\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B152829-C309-4B66-B725-0F6A64D54E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>aluno_id</t>
-  </si>
-  <si>
-    <t>created_at</t>
-  </si>
-  <si>
-    <t>nome</t>
-  </si>
-  <si>
-    <t>updated_at</t>
-  </si>
-  <si>
-    <t>curso_id</t>
-  </si>
-  <si>
-    <t>matricula_id</t>
-  </si>
-  <si>
-    <t>c67b4ea9-8683-49fe-bbd0-2b6747bf4c7a</t>
-  </si>
-  <si>
-    <t>Cleber</t>
-  </si>
-  <si>
-    <t>dc0a6e4b-ff9b-4788-a373-c62ee913e99c</t>
-  </si>
-  <si>
-    <t>06aed628-8817-4d4a-bf9b-7b5878844305</t>
-  </si>
-  <si>
-    <t>f176015e-4375-402a-88dd-437eedb0c857</t>
-  </si>
-  <si>
-    <t>Jorge</t>
-  </si>
-  <si>
-    <t>48c6389c-7929-4bd6-a062-3f0542bd597a</t>
-  </si>
-  <si>
-    <t>d532a36f-9876-474d-914f-7d412efe2472</t>
-  </si>
-  <si>
-    <t>2e24dfd9-cf26-4294-b36a-3e40bce302c9</t>
-  </si>
-  <si>
-    <t>Lamar</t>
-  </si>
-  <si>
-    <t>11d8663c-2180-4d4c-94e6-d387090cbc0c</t>
-  </si>
-  <si>
-    <t>bf21728a-8a7e-4552-a492-b30503855dd9</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -114,44 +48,95 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -439,108 +424,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45.85546875" customWidth="1"/>
-    <col min="7" max="7" width="36.28515625" customWidth="1"/>
+    <col width="36" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>aluno_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>created_at</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>updated_at</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>curso_id</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>matricula_id</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45658.64822246808</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2">
-        <v>45658.648275614112</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>c67b4ea9-8683-49fe-bbd0-2b6747bf4c7a</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>45658.64822246528</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cleber</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>45658.64827561343</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>dc0a6e4b-ff9b-4788-a373-c62ee913e99c</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>06aed628-8817-4d4a-bf9b-7b5878844305</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45658.648707059263</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2">
-        <v>45658.649255831922</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>f176015e-4375-402a-88dd-437eedb0c857</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>45658.64870706019</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Jorge</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>45658.64925583333</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>48c6389c-7929-4bd6-a062-3f0542bd597a</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>d532a36f-9876-474d-914f-7d412efe2472</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2">
-        <v>45658.842175216967</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2">
-        <v>45658.842175216967</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2e24dfd9-cf26-4294-b36a-3e40bce302c9</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>45658.84217521991</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Lamar</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>45658.84217521991</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>11d8663c-2180-4d4c-94e6-d387090cbc0c</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>bf21728a-8a7e-4552-a492-b30503855dd9</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refatorando o codigo para cada uma das etapas
</commit_message>
<xml_diff>
--- a/df_tabela.xlsx
+++ b/df_tabela.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,39 +437,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="36" customWidth="1" min="1" max="1"/>
+    <col width="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>aluno_id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>created_at</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>nome</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>updated_at</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>curso_id</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>matricula_id</t>
-        </is>
+      <c r="A1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -553,6 +541,34 @@
       <c r="F4" t="inlineStr">
         <is>
           <t>bf21728a-8a7e-4552-a492-b30503855dd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>e350f4f4-91d9-47d2-8ada-c2c35e6b7926</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>45660.77291162037</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cj</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>45660.77291162037</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>11d8663c-2180-4d4c-94e6-d387090cbc0c</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>d4e541ab-52c8-4d0d-a28f-cd5f3856aec6</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Separando o arquivo main das funcoes
</commit_message>
<xml_diff>
--- a/df_tabela.xlsx
+++ b/df_tabela.xlsx
@@ -437,27 +437,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="1" customWidth="1" min="1" max="1"/>
+    <col width="36" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>5</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>aluno_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>created_at</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>updated_at</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>curso_id</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>matricula_id</t>
+        </is>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Ajustando tamanho da tabela conforme o tamanho dos dados
</commit_message>
<xml_diff>
--- a/df_tabela.xlsx
+++ b/df_tabela.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +437,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="36" customWidth="1" min="1" max="1"/>
+    <col width="37" customWidth="1" min="1" max="1"/>
+    <col width="27" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="37" customWidth="1" min="5" max="5"/>
+    <col width="37" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -581,6 +586,34 @@
       <c r="F5" t="inlineStr">
         <is>
           <t>d4e541ab-52c8-4d0d-a28f-cd5f3856aec6</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>8ff8d609-d981-4dd6-9bb0-363ca82a9f79</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>45660.81807527778</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Big Smoke</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>45660.81807527778</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>11d8663c-2180-4d4c-94e6-d387090cbc0c</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>d7a7a28b-fbb2-4190-b2fb-fc139d0f34ae</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Relatorio de medias doas alunos funcionando
</commit_message>
<xml_diff>
--- a/df_tabela.xlsx
+++ b/df_tabela.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,184 +425,78 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="19" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>aluno_id</t>
+          <t>nome</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>created_at</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>nome</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>updated_at</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>curso_id</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>matricula_id</t>
+          <t>Média das Notas</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>c67b4ea9-8683-49fe-bbd0-2b6747bf4c7a</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>45658.64822246808</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Cleber</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>45658.64827561411</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>dc0a6e4b-ff9b-4788-a373-c62ee913e99c</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>06aed628-8817-4d4a-bf9b-7b5878844305</t>
-        </is>
+          <t>Big Smoke</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>6.083333333333333</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>f176015e-4375-402a-88dd-437eedb0c857</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>45658.64870705926</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Jorge</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>45658.64925583192</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>48c6389c-7929-4bd6-a062-3f0542bd597a</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>d532a36f-9876-474d-914f-7d412efe2472</t>
-        </is>
+          <t>Cj</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2e24dfd9-cf26-4294-b36a-3e40bce302c9</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>45658.84217521697</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Lamar</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>45658.84217521697</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>11d8663c-2180-4d4c-94e6-d387090cbc0c</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>bf21728a-8a7e-4552-a492-b30503855dd9</t>
-        </is>
+          <t>Cleber</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1.166666666666667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>e350f4f4-91d9-47d2-8ada-c2c35e6b7926</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>45660.77291162009</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Cj</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>45660.77291162009</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>11d8663c-2180-4d4c-94e6-d387090cbc0c</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>d4e541ab-52c8-4d0d-a28f-cd5f3856aec6</t>
-        </is>
+          <t>Jorge</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>8ff8d609-d981-4dd6-9bb0-363ca82a9f79</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>45660.8180752805</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Big Smoke</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>45660.8180752805</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>11d8663c-2180-4d4c-94e6-d387090cbc0c</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>d7a7a28b-fbb2-4190-b2fb-fc139d0f34ae</t>
-        </is>
+          <t>Lamar</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>